<commit_message>
SetUncagingPosition is sent before each step
</commit_message>
<xml_diff>
--- a/io_API.xlsx
+++ b/io_API.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
   <si>
     <t>Command</t>
   </si>
@@ -288,6 +288,36 @@
   </si>
   <si>
     <t>do uncaging at specific position signified by pixel value in image</t>
+  </si>
+  <si>
+    <t>CustomCommand</t>
+  </si>
+  <si>
+    <t>CustomCommandReceived</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>CustomCommand,page_acq</t>
+  </si>
+  <si>
+    <t>send a custom command to imaging program immediately before executing a step</t>
+  </si>
+  <si>
+    <t>UncagingLocation</t>
+  </si>
+  <si>
+    <t>SetUncagingLocation</t>
+  </si>
+  <si>
+    <t>SetUncagingLocation,37,42</t>
+  </si>
+  <si>
+    <t>sends an uncaging location without actually uncaging</t>
+  </si>
+  <si>
+    <t>sent as an answer to SetUncagingLocation</t>
   </si>
 </sst>
 </file>
@@ -615,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -822,226 +852,276 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>60</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>62</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>13</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>87</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A20:E34">
+  <sortState ref="A21:E35">
     <sortCondition ref="A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replaced StageMoveDone with SetMotorPositionDone
</commit_message>
<xml_diff>
--- a/io_API.xlsx
+++ b/io_API.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smirnovm\Documents\ProgrammingProjects\SpineTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasudalab.MPFI\Documents\Software\SpineTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>Command</t>
   </si>
@@ -50,9 +50,6 @@
     <t>x, y, z</t>
   </si>
   <si>
-    <t>StageMoveDone,1,34.2,-2</t>
-  </si>
-  <si>
     <t>CurrentPosition</t>
   </si>
   <si>
@@ -318,6 +315,12 @@
   </si>
   <si>
     <t>sent as an answer to SetUncagingLocation</t>
+  </si>
+  <si>
+    <t>SetMotorPositionDone</t>
+  </si>
+  <si>
+    <t>SetMotorPositionDone,1,34.2,-2</t>
   </si>
 </sst>
 </file>
@@ -648,24 +651,24 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="38.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -687,437 +690,437 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
         <v>63</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
         <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>51</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>61</v>
       </c>
-      <c r="C35" t="s">
-        <v>62</v>
-      </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
         <v>88</v>
       </c>
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>91</v>
       </c>
-      <c r="D36" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>